<commit_message>
added quarters with OO
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@863 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/Agendas/201305 WGM FHIR Agenda.xlsx
+++ b/documents/Agendas/201305 WGM FHIR Agenda.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
   <si>
     <t>Clinical Genomics</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Work Group</t>
+  </si>
+  <si>
+    <t>GG</t>
   </si>
 </sst>
 </file>
@@ -338,18 +341,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -368,6 +359,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,17 +675,17 @@
   <dimension ref="A1:X33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="4.42578125" customWidth="1"/>
     <col min="10" max="10" width="4.42578125" style="9" customWidth="1"/>
     <col min="11" max="13" width="4.42578125" customWidth="1"/>
@@ -697,37 +700,37 @@
     <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="13" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="10" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="10" t="s">
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="10" t="s">
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="11"/>
+      <c r="X1" s="19"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -739,10 +742,10 @@
       <c r="C2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="11" t="s">
         <v>58</v>
       </c>
       <c r="F2" s="6" t="s">
@@ -813,8 +816,8 @@
       <c r="C3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -823,11 +826,11 @@
         <v>47</v>
       </c>
       <c r="N3" s="8"/>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="16" t="s">
         <v>48</v>
       </c>
       <c r="S3" s="8"/>
-      <c r="W3" s="21" t="s">
+      <c r="W3" s="17" t="s">
         <v>47</v>
       </c>
       <c r="X3" s="5"/>
@@ -842,19 +845,19 @@
       <c r="C4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="8"/>
       <c r="N4" s="8"/>
-      <c r="R4" s="20" t="s">
+      <c r="R4" s="16" t="s">
         <v>47</v>
       </c>
       <c r="S4" s="8"/>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="17" t="s">
         <v>47</v>
       </c>
       <c r="X4" s="5"/>
@@ -867,17 +870,17 @@
         <v>13</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="8"/>
       <c r="N5" s="8"/>
-      <c r="R5" s="20"/>
+      <c r="R5" s="16"/>
       <c r="S5" s="8"/>
-      <c r="W5" s="21"/>
+      <c r="W5" s="17"/>
       <c r="X5" s="5"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -890,19 +893,19 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="12">
         <v>1</v>
       </c>
-      <c r="E6" s="16"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="8"/>
       <c r="N6" s="8"/>
-      <c r="R6" s="20"/>
+      <c r="R6" s="16"/>
       <c r="S6" s="8"/>
-      <c r="W6" s="21"/>
+      <c r="W6" s="17"/>
       <c r="X6" s="5"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -915,19 +918,19 @@
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="8"/>
       <c r="N7" s="8"/>
-      <c r="R7" s="20"/>
+      <c r="R7" s="16"/>
       <c r="S7" s="8"/>
-      <c r="W7" s="21"/>
+      <c r="W7" s="17"/>
       <c r="X7" s="5"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -940,8 +943,8 @@
       <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
         <v>63</v>
       </c>
       <c r="F8" s="5"/>
@@ -950,9 +953,9 @@
       <c r="I8" s="5"/>
       <c r="J8" s="8"/>
       <c r="N8" s="8"/>
-      <c r="R8" s="20"/>
+      <c r="R8" s="16"/>
       <c r="S8" s="8"/>
-      <c r="W8" s="21"/>
+      <c r="W8" s="17"/>
       <c r="X8" s="5"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -965,17 +968,17 @@
       <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
       <c r="N9" s="8"/>
-      <c r="R9" s="20"/>
+      <c r="R9" s="16"/>
       <c r="S9" s="8"/>
-      <c r="W9" s="21"/>
+      <c r="W9" s="17"/>
       <c r="X9" s="5"/>
     </row>
     <row r="10" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -988,10 +991,10 @@
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="12" t="s">
         <v>61</v>
       </c>
       <c r="F10" s="5"/>
@@ -1000,9 +1003,9 @@
       <c r="I10" s="5"/>
       <c r="J10" s="8"/>
       <c r="N10" s="8"/>
-      <c r="R10" s="20"/>
+      <c r="R10" s="16"/>
       <c r="S10" s="8"/>
-      <c r="W10" s="21"/>
+      <c r="W10" s="17"/>
       <c r="X10" s="5"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -1015,17 +1018,17 @@
       <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="R11" s="20"/>
+      <c r="R11" s="16"/>
       <c r="S11" s="8"/>
-      <c r="W11" s="21"/>
+      <c r="W11" s="17"/>
       <c r="X11" s="5"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -1038,8 +1041,8 @@
       <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="5" t="s">
         <v>47</v>
       </c>
@@ -1054,11 +1057,11 @@
       </c>
       <c r="J12" s="8"/>
       <c r="N12" s="8"/>
-      <c r="R12" s="20"/>
+      <c r="R12" s="16"/>
       <c r="S12" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="W12" s="21"/>
+      <c r="W12" s="17"/>
       <c r="X12" s="5" t="s">
         <v>47</v>
       </c>
@@ -1073,19 +1076,19 @@
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="16"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
       <c r="N13" s="8"/>
-      <c r="R13" s="20"/>
+      <c r="R13" s="16"/>
       <c r="S13" s="8"/>
-      <c r="W13" s="21"/>
+      <c r="W13" s="17"/>
       <c r="X13" s="5"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1098,19 +1101,19 @@
       <c r="C14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
       <c r="N14" s="8"/>
-      <c r="R14" s="20"/>
+      <c r="R14" s="16"/>
       <c r="S14" s="8"/>
-      <c r="W14" s="21"/>
+      <c r="W14" s="17"/>
       <c r="X14" s="5"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -1123,19 +1126,19 @@
       <c r="C15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="16"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
       <c r="N15" s="8"/>
-      <c r="R15" s="20"/>
+      <c r="R15" s="16"/>
       <c r="S15" s="8"/>
-      <c r="W15" s="21"/>
+      <c r="W15" s="17"/>
       <c r="X15" s="5"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -1143,24 +1146,24 @@
         <v>16</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="16"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
       <c r="N16" s="8"/>
-      <c r="R16" s="20"/>
+      <c r="R16" s="16"/>
       <c r="S16" s="8"/>
-      <c r="W16" s="21"/>
+      <c r="W16" s="17"/>
       <c r="X16" s="5"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
@@ -1173,10 +1176,10 @@
       <c r="C17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="16"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5" t="s">
@@ -1187,9 +1190,9 @@
       </c>
       <c r="J17" s="8"/>
       <c r="N17" s="8"/>
-      <c r="R17" s="20"/>
+      <c r="R17" s="16"/>
       <c r="S17" s="8"/>
-      <c r="W17" s="21"/>
+      <c r="W17" s="17"/>
       <c r="X17" s="5"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
@@ -1202,10 +1205,10 @@
       <c r="C18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="12" t="s">
         <v>59</v>
       </c>
       <c r="F18" s="5"/>
@@ -1214,9 +1217,9 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
       <c r="N18" s="8"/>
-      <c r="R18" s="20"/>
+      <c r="R18" s="16"/>
       <c r="S18" s="8"/>
-      <c r="W18" s="21"/>
+      <c r="W18" s="17"/>
       <c r="X18" s="5"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
@@ -1229,19 +1232,19 @@
       <c r="C19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="12"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
       <c r="N19" s="8"/>
-      <c r="R19" s="20"/>
+      <c r="R19" s="16"/>
       <c r="S19" s="8"/>
-      <c r="W19" s="21"/>
+      <c r="W19" s="17"/>
       <c r="X19" s="5"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
@@ -1254,8 +1257,8 @@
       <c r="C20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="5" t="s">
         <v>47</v>
       </c>
@@ -1270,11 +1273,11 @@
       </c>
       <c r="J20" s="8"/>
       <c r="N20" s="8"/>
-      <c r="R20" s="20"/>
+      <c r="R20" s="16"/>
       <c r="S20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="W20" s="21"/>
+      <c r="W20" s="17"/>
       <c r="X20" s="5" t="s">
         <v>47</v>
       </c>
@@ -1289,19 +1292,25 @@
       <c r="C21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="16"/>
+      <c r="D21" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="12"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
       <c r="N21" s="8"/>
-      <c r="R21" s="20"/>
+      <c r="O21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R21" s="16"/>
       <c r="S21" s="8"/>
-      <c r="W21" s="21"/>
+      <c r="T21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W21" s="17"/>
       <c r="X21" s="5"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
@@ -1314,19 +1323,19 @@
       <c r="C22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="12"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="8"/>
       <c r="N22" s="8"/>
-      <c r="R22" s="20"/>
+      <c r="R22" s="16"/>
       <c r="S22" s="8"/>
-      <c r="W22" s="21"/>
+      <c r="W22" s="17"/>
       <c r="X22" s="5"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
@@ -1339,19 +1348,19 @@
       <c r="C23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="12"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="8"/>
       <c r="N23" s="8"/>
-      <c r="R23" s="20"/>
+      <c r="R23" s="16"/>
       <c r="S23" s="8"/>
-      <c r="W23" s="21"/>
+      <c r="W23" s="17"/>
       <c r="X23" s="5"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
@@ -1364,19 +1373,19 @@
       <c r="C24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="12"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="8"/>
       <c r="N24" s="8"/>
-      <c r="R24" s="20"/>
+      <c r="R24" s="16"/>
       <c r="S24" s="8"/>
-      <c r="W24" s="21"/>
+      <c r="W24" s="17"/>
       <c r="X24" s="5"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -1389,19 +1398,19 @@
       <c r="C25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="12"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="8"/>
       <c r="N25" s="8"/>
-      <c r="R25" s="20"/>
+      <c r="R25" s="16"/>
       <c r="S25" s="8"/>
-      <c r="W25" s="21"/>
+      <c r="W25" s="17"/>
       <c r="X25" s="5"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
@@ -1414,17 +1423,17 @@
       <c r="C26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="8"/>
       <c r="N26" s="8"/>
-      <c r="R26" s="20"/>
+      <c r="R26" s="16"/>
       <c r="S26" s="8"/>
-      <c r="W26" s="21"/>
+      <c r="W26" s="17"/>
       <c r="X26" s="5"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
@@ -1437,17 +1446,17 @@
       <c r="C27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="R27" s="20"/>
+      <c r="R27" s="16"/>
       <c r="S27" s="8"/>
-      <c r="W27" s="21"/>
+      <c r="W27" s="17"/>
       <c r="X27" s="5"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
@@ -1460,10 +1469,10 @@
       <c r="C28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="12" t="s">
         <v>60</v>
       </c>
       <c r="F28" s="5"/>
@@ -1472,9 +1481,9 @@
       <c r="I28" s="5"/>
       <c r="J28" s="8"/>
       <c r="N28" s="8"/>
-      <c r="R28" s="20"/>
+      <c r="R28" s="16"/>
       <c r="S28" s="8"/>
-      <c r="W28" s="21"/>
+      <c r="W28" s="17"/>
       <c r="X28" s="5"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
@@ -1487,10 +1496,10 @@
       <c r="C29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="12" t="s">
         <v>60</v>
       </c>
       <c r="F29" s="5"/>
@@ -1499,9 +1508,9 @@
       <c r="I29" s="5"/>
       <c r="J29" s="8"/>
       <c r="N29" s="8"/>
-      <c r="R29" s="20"/>
+      <c r="R29" s="16"/>
       <c r="S29" s="8"/>
-      <c r="W29" s="21"/>
+      <c r="W29" s="17"/>
       <c r="X29" s="5"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
@@ -1514,19 +1523,19 @@
       <c r="C30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="16"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="8"/>
       <c r="N30" s="8"/>
-      <c r="R30" s="20"/>
+      <c r="R30" s="16"/>
       <c r="S30" s="8"/>
-      <c r="W30" s="21"/>
+      <c r="W30" s="17"/>
       <c r="X30" s="5"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
@@ -1539,10 +1548,10 @@
       <c r="C31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="12" t="s">
         <v>62</v>
       </c>
       <c r="F31" s="5"/>
@@ -1551,9 +1560,9 @@
       <c r="I31" s="5"/>
       <c r="J31" s="8"/>
       <c r="N31" s="8"/>
-      <c r="R31" s="20"/>
+      <c r="R31" s="16"/>
       <c r="S31" s="8"/>
-      <c r="W31" s="21"/>
+      <c r="W31" s="17"/>
       <c r="X31" s="5"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
@@ -1566,17 +1575,17 @@
       <c r="C32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="8"/>
       <c r="N32" s="8"/>
-      <c r="R32" s="20"/>
+      <c r="R32" s="16"/>
       <c r="S32" s="8"/>
-      <c r="W32" s="21"/>
+      <c r="W32" s="17"/>
       <c r="X32" s="5"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
@@ -1589,22 +1598,22 @@
       <c r="C33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="18"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="8"/>
       <c r="N33" s="8"/>
-      <c r="O33" s="14" t="s">
+      <c r="O33" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="R33" s="20"/>
+      <c r="R33" s="16"/>
       <c r="S33" s="8"/>
-      <c r="W33" s="21"/>
+      <c r="W33" s="17"/>
       <c r="X33" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added second CGIT session
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@914 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/Agendas/201305 WGM FHIR Agenda.xlsx
+++ b/documents/Agendas/201305 WGM FHIR Agenda.xlsx
@@ -343,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -394,6 +394,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,7 +705,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +949,7 @@
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="25" t="s">
         <v>55</v>
       </c>
       <c r="E7" s="13"/>
@@ -955,6 +958,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="8"/>
+      <c r="K7" s="10"/>
       <c r="N7" s="8"/>
       <c r="Q7" s="10" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Added sessions for PA and Mobile Health
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@946 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/documents/Agendas/201305 WGM FHIR Agenda.xlsx
+++ b/documents/Agendas/201305 WGM FHIR Agenda.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Live\HL7\FHIR\Fhir SVN\documents\Agendas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14565"/>
   </bookViews>
@@ -16,10 +21,35 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Hugh Glover</author>
     <author>Lloyd McKenzie</author>
   </authors>
   <commentList>
-    <comment ref="D25" authorId="0">
+    <comment ref="K22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Hugh Glover:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Waiting for confirmation from PA</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="78">
   <si>
     <t>Clinical Genomics</t>
   </si>
@@ -279,13 +309,16 @@
   </si>
   <si>
     <t>1+</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,8 +354,21 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,6 +494,10 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,9 +510,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,6 +519,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -514,7 +570,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -549,7 +605,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -764,7 +820,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,35 +844,35 @@
       <c r="C1" s="6"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="22" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="22" t="s">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="22" t="s">
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="22" t="s">
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="23"/>
+      <c r="X1" s="25"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -983,7 +1039,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="22">
         <v>1</v>
       </c>
       <c r="E6" s="12"/>
@@ -1371,6 +1427,9 @@
       <c r="K19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="8"/>
+      <c r="P19" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="R19" s="16"/>
       <c r="S19" s="8"/>
       <c r="W19" s="17"/>
@@ -1462,6 +1521,12 @@
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="8"/>
+      <c r="K22" t="s">
+        <v>77</v>
+      </c>
+      <c r="L22" t="s">
+        <v>77</v>
+      </c>
       <c r="N22" s="8"/>
       <c r="R22" s="16"/>
       <c r="S22" s="8"/>

</xml_diff>